<commit_message>
4 scenario are added 9, 10, 24, 25
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="162">
   <si>
     <t xml:space="preserve">TestName</t>
   </si>
@@ -345,10 +345,34 @@
     <t xml:space="preserve">Edit_LossHistory_LossAmount</t>
   </si>
   <si>
+    <t xml:space="preserve">Layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reinstatement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BuildingYear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buildings</t>
+  </si>
+  <si>
     <t xml:space="preserve">User should be able to Assign Underwriter &amp; UW Team for selected Contract Number using action "ASSIGN UNDERWRITER".</t>
   </si>
   <si>
-    <t xml:space="preserve">783</t>
+    <t xml:space="preserve">719</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to REASSIGN Underwriter &amp; UW Team for selected Contract Number using action "REASSIGN UNDERWRITER".</t>
@@ -357,12 +381,15 @@
     <t xml:space="preserve">Canada</t>
   </si>
   <si>
-    <t xml:space="preserve">User should be able to update "Firm Order Term Details" for selected Contract Number using action "UPDATE FIRM ORDER TERMS"(Provided User already sent the mail "Firm Order Terms" to ProcessModel ID)</t>
+    <t xml:space="preserve">User should be able to do "Actuarial Assignment" or "Legal Assignment" for selected Contract Number using action "ACTUARIAL ASSIGNMENT" or  "LEGAL ASSIGNMENT".</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to send "Authorization Email" for selected Contract Number using action "SEND AUTHORIZATION EMAIL".</t>
   </si>
   <si>
+    <t xml:space="preserve">665</t>
+  </si>
+  <si>
     <t xml:space="preserve">This is a test wording Proposal text.</t>
   </si>
   <si>
@@ -396,12 +423,18 @@
     <t xml:space="preserve">User should be able to do "UPFRONT ANALYSIS" for selected Contract Number using action "UPFRONT ANALYSIS"</t>
   </si>
   <si>
+    <t xml:space="preserve">712</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_007</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to "Update Written Line" for selected Contract Number using action "UPDATE WRITTEN LINES"</t>
   </si>
   <si>
+    <t xml:space="preserve">536</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
@@ -411,10 +444,16 @@
     <t xml:space="preserve">User should be able to "Update Pricing Structure Overview" for selected Contract Number using action "PRICING STRUCTURE OVERVIEW</t>
   </si>
   <si>
+    <t xml:space="preserve">689</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_009</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to update "Considerations" for selected Contract Number using action "UPDATE OVERALL CONSIDERATIONS"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">619</t>
   </si>
   <si>
     <t xml:space="preserve">TC_010</t>
@@ -430,41 +469,49 @@
     <t xml:space="preserve">#27 User should be able to Add/ Delete Records and Update Details for "Loss History" and "SAVE CHANGES" for selected Contract Number using button "EDIT" located at top Right corner of the page.(Loss History - Panel below Case Details)</t>
   </si>
   <si>
+    <t xml:space="preserve">710</t>
+  </si>
+  <si>
     <t xml:space="preserve">test loss history2</t>
   </si>
   <si>
     <t xml:space="preserve">TC_012</t>
   </si>
   <si>
-    <t xml:space="preserve">#33 User should be able to take "Authorization Decision" as APPROVE for selected Contract Number using action "AUTHORIZATION DECISION"
-#34 User should be able to take "Authorization Decision" as REJECT for selected Contract Number using action "AUTHORIZATION DECISION"</t>
+    <t xml:space="preserve">User should be able to Add/ Delete Records and Update Details for "Program Structure" and "SAVE CHANGES" for selected Contract Number using button "EDIT" located at top Right corner of the page.(Program Structure - Panel below Case Details)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st Layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property Test New XoL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2800000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">185000000</t>
   </si>
   <si>
     <t xml:space="preserve">TC_013</t>
   </si>
   <si>
-    <t xml:space="preserve">User should be able to do "Program Authorization" for selected Contract Number using action "PROCEED TO NEXT LEVEL AUTHORIZATION"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to send "Signed Contract" for selected Contract Number using action "SEND SIGNED CONTRACT"(Provided User already sent the "Signing Contract" to ProcessModel ID with attachment: REINSURANCE CONTRACT SIGNING PAGE &amp; thereafter completing Action SIGN CONTRACT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to "Add Quotation Details" for selected Contract Number using action "ADD QUOTATION"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to send "Non Binding Refusal Email" for selected Contract Number using action "SEND NON BINDING REFUSAL EMAIL".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_017</t>
+    <t xml:space="preserve">User should be able to Add/ Delete Records and Update Details for "Building Year" and "SAVE CHANGES" for selected Contract Number using button "EDIT" located at top Right corner of the page.(Building Year- Panel below Case Details)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1996 – 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">029</t>
   </si>
 </sst>
 </file>
@@ -618,7 +665,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -737,6 +784,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -925,8 +976,8 @@
   </sheetPr>
   <dimension ref="A1:AO1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="C10 A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1210,7 +1261,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="1" sqref="C10 B6"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1300,7 +1351,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="C10 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1375,13 +1426,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C10 B1"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.57"/>
   </cols>
@@ -1474,10 +1525,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C10" activeCellId="0" sqref="C10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1487,8 +1538,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="2" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1552,16 +1605,40 @@
       <c r="T1" s="25" t="s">
         <v>105</v>
       </c>
+      <c r="U1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>72</v>
@@ -1577,48 +1654,48 @@
         <v>74</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1626,182 +1703,172 @@
         <v>56</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="L5" s="27" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="M5" s="27" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="122.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>107</v>
-      </c>
+      <c r="A11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="U11" s="10"/>
+      <c r="W11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="R12" s="23" t="n">
+      <c r="A12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="R12" s="24" t="n">
         <v>2027</v>
       </c>
-      <c r="S12" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="T12" s="23" t="n">
+      <c r="S12" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="T12" s="24" t="n">
         <v>4563645</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>135</v>
+    <row r="13" customFormat="false" ht="36.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="V13" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="W13" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="X13" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y13" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z13" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="39.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="27.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>145</v>
+        <v>158</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="AA14" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB14" s="20" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actuarial building and program structure feature file updated
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="162">
   <si>
     <t xml:space="preserve">TestName</t>
   </si>
@@ -345,10 +345,34 @@
     <t xml:space="preserve">Edit_LossHistory_LossAmount</t>
   </si>
   <si>
+    <t xml:space="preserve">Layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program Type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Limit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reinstatement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subject Premium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BuildingYear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buildings</t>
+  </si>
+  <si>
     <t xml:space="preserve">User should be able to Assign Underwriter &amp; UW Team for selected Contract Number using action "ASSIGN UNDERWRITER".</t>
   </si>
   <si>
-    <t xml:space="preserve">785</t>
+    <t xml:space="preserve">719</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to REASSIGN Underwriter &amp; UW Team for selected Contract Number using action "REASSIGN UNDERWRITER".</t>
@@ -357,12 +381,15 @@
     <t xml:space="preserve">Canada</t>
   </si>
   <si>
-    <t xml:space="preserve">User should be able to update "Firm Order Term Details" for selected Contract Number using action "UPDATE FIRM ORDER TERMS"(Provided User already sent the mail "Firm Order Terms" to ProcessModel ID)</t>
+    <t xml:space="preserve">User should be able to do "Actuarial Assignment" or "Legal Assignment" for selected Contract Number using action "ACTUARIAL ASSIGNMENT" or  "LEGAL ASSIGNMENT".</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to send "Authorization Email" for selected Contract Number using action "SEND AUTHORIZATION EMAIL".</t>
   </si>
   <si>
+    <t xml:space="preserve">665</t>
+  </si>
+  <si>
     <t xml:space="preserve">This is a test wording Proposal text.</t>
   </si>
   <si>
@@ -396,12 +423,18 @@
     <t xml:space="preserve">User should be able to do "UPFRONT ANALYSIS" for selected Contract Number using action "UPFRONT ANALYSIS"</t>
   </si>
   <si>
+    <t xml:space="preserve">712</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_007</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to "Update Written Line" for selected Contract Number using action "UPDATE WRITTEN LINES"</t>
   </si>
   <si>
+    <t xml:space="preserve">536</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
@@ -411,10 +444,16 @@
     <t xml:space="preserve">User should be able to "Update Pricing Structure Overview" for selected Contract Number using action "PRICING STRUCTURE OVERVIEW</t>
   </si>
   <si>
+    <t xml:space="preserve">689</t>
+  </si>
+  <si>
     <t xml:space="preserve">TC_009</t>
   </si>
   <si>
     <t xml:space="preserve">User should be able to update "Considerations" for selected Contract Number using action "UPDATE OVERALL CONSIDERATIONS"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">619</t>
   </si>
   <si>
     <t xml:space="preserve">TC_010</t>
@@ -430,44 +469,49 @@
     <t xml:space="preserve">#27 User should be able to Add/ Delete Records and Update Details for "Loss History" and "SAVE CHANGES" for selected Contract Number using button "EDIT" located at top Right corner of the page.(Loss History - Panel below Case Details)</t>
   </si>
   <si>
+    <t xml:space="preserve">710</t>
+  </si>
+  <si>
     <t xml:space="preserve">test loss history2</t>
   </si>
   <si>
     <t xml:space="preserve">TC_012</t>
   </si>
   <si>
-    <t xml:space="preserve">#33 User should be able to take "Authorization Decision" as APPROVE for selected Contract Number using action "AUTHORIZATION DECISION"
-#34 User should be able to take "Authorization Decision" as REJECT for selected Contract Number using action "AUTHORIZATION DECISION"</t>
+    <t xml:space="preserve">User should be able to Add/ Delete Records and Update Details for "Program Structure" and "SAVE CHANGES" for selected Contract Number using button "EDIT" located at top Right corner of the page.(Program Structure - Panel below Case Details)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1st Layer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Property Test New XoL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2800000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16100000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1@100%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">185000000</t>
   </si>
   <si>
     <t xml:space="preserve">TC_013</t>
   </si>
   <si>
-    <t xml:space="preserve">User should be able to do "Program Authorization" for selected Contract Number using action "PROCEED TO NEXT LEVEL AUTHORIZATION"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to send "Signed Contract" for selected Contract Number using action "SEND SIGNED CONTRACT"(Provided User already sent the "Signing Contract" to ProcessModel ID with attachment: REINSURANCE CONTRACT SIGNING PAGE &amp; thereafter completing Action SIGN CONTRACT)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to "Add Quotation Details" for selected Contract Number using action "ADD QUOTATION"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_016</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to send "Non Binding Refusal Email" for selected Contract Number using action "SEND NON BINDING REFUSAL EMAIL".</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TC_017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User should be able to send "Non Binding Refusal Email" for selected Contract Number using action "SEND NON BINDING AUTHORIZATION  EMAIL".</t>
+    <t xml:space="preserve">User should be able to Add/ Delete Records and Update Details for "Building Year" and "SAVE CHANGES" for selected Contract Number using button "EDIT" located at top Right corner of the page.(Building Year- Panel below Case Details)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1996 – 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">029</t>
   </si>
 </sst>
 </file>
@@ -621,7 +665,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -740,6 +784,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -928,7 +976,7 @@
   </sheetPr>
   <dimension ref="A1:AO1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1378,13 +1426,13 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="G19" activeCellId="0" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="14.25" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="27.57"/>
   </cols>
@@ -1477,10 +1525,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T18"/>
+  <dimension ref="A1:AB14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1490,8 +1538,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.65"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="16" style="2" width="12.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="16.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="14.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="32" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1555,16 +1605,40 @@
       <c r="T1" s="25" t="s">
         <v>105</v>
       </c>
+      <c r="U1" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="V1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="W1" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="X1" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="Y1" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z1" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
         <v>71</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>72</v>
@@ -1580,48 +1654,48 @@
         <v>74</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="10" t="s">
-        <v>87</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>75</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-    </row>
-    <row r="5" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>76</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
@@ -1629,188 +1703,172 @@
         <v>56</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="J5" s="27" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="K5" s="27" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="L5" s="27" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="M5" s="27" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="O6" s="15" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>107</v>
+        <v>132</v>
       </c>
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
     </row>
     <row r="8" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>107</v>
+        <v>135</v>
       </c>
       <c r="P8" s="20" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="Q8" s="20" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="23" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>128</v>
+        <v>140</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>107</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="122.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="B11" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>107</v>
-      </c>
+      <c r="A11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>144</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="U11" s="10"/>
+      <c r="W11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="36.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="R12" s="23" t="n">
+      <c r="A12" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>146</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="R12" s="24" t="n">
         <v>2027</v>
       </c>
-      <c r="S12" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="T12" s="23" t="n">
+      <c r="S12" s="24" t="s">
+        <v>148</v>
+      </c>
+      <c r="T12" s="24" t="n">
         <v>4563645</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="58.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
-        <v>135</v>
+    <row r="13" customFormat="false" ht="36.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>150</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="U13" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="V13" s="23" t="s">
+        <v>153</v>
+      </c>
+      <c r="W13" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="X13" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="Y13" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z13" s="20" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="39.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C15" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="23.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="27.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>144</v>
-      </c>
-      <c r="C17" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B18" s="23" t="s">
-        <v>146</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>107</v>
+        <v>158</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="X14" s="30"/>
+      <c r="Y14" s="30"/>
+      <c r="AA14" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="AB14" s="20" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>